<commit_message>
AIP-1541 AIP-1546 changed the code for IDME cabling 3U/1U using IDM+ code
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_16Channel/1U3I.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_16Channel/1U3I.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55FE7DA-D58C-4095-9275-7B4228CE6BE5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACC1C3F-8930-4968-AFFC-159B67BD90AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeviceInfo" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="128">
   <si>
     <t>Channel</t>
   </si>
@@ -401,7 +401,13 @@
     <t>10.75.58.66</t>
   </si>
   <si>
-    <t>sn414638044_3U_15I.cal</t>
+    <t>3U_13I.cal</t>
+  </si>
+  <si>
+    <t>Channel 17</t>
+  </si>
+  <si>
+    <t>Channel 18</t>
   </si>
 </sst>
 </file>
@@ -724,8 +730,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,10 +766,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AB21"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22:AB23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,6 +1467,16 @@
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="W21" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W23" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1568,8 +1584,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,7 +1932,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AIP-1584 AIP-1587 mds file updated for Test Result publish
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_16Channel/1U3I.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_16Channel/1U3I.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACC1C3F-8930-4968-AFFC-159B67BD90AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2567F1C4-DCDA-4013-9CCF-9D9EE04CD972}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeviceInfo" sheetId="3" r:id="rId1"/>
@@ -730,7 +730,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1931,7 +1931,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>